<commit_message>
Upload image for new report function done
</commit_message>
<xml_diff>
--- a/policedatabase.xlsx
+++ b/policedatabase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\Desktop\CS project\face rec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\Documents\GitHub\ver_05_11_clone\le_csproject-2904-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0C07751-2F95-43C2-BE1A-96A87C10FCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5A4B53-CBEF-47D0-A5D6-449C3AF7AF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0C697BBE-DCA3-4054-B14F-BD5BD2CE263D}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN1.jpg</t>
-  </si>
-  <si>
     <t>Kanye West</t>
   </si>
   <si>
@@ -119,31 +116,34 @@
     <t>Kylie Jenner</t>
   </si>
   <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN2.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN3.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN4.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN5.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN6.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN7.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN8.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN9.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\ayush\Desktop\CS project\MPIN_pictures\TN10.jpg</t>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN1.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN2.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN3.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN4.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN5.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN6.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN7.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN8.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN9.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\ayush\Desktop\CS PROJECT\MPIN_pictures\TN10.jpg</t>
   </si>
 </sst>
 </file>
@@ -185,13 +185,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +508,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -524,177 +523,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>44126</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="3">
-        <v>44126</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>